<commit_message>
session 9 and 10 added
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anisa Spring\course files\anisa-spring-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7761E6-4ACC-43C6-B159-A6B52E1AC5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500CDC3-19F8-4721-A055-3DF116E18CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="2" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="188">
   <si>
     <t>Session</t>
   </si>
@@ -653,9 +653,6 @@
     <t>Spring Form jsp Tags</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>introduced in Spring 2.0
 bundled in Spring-mvc.jar
 advantages:
@@ -682,6 +679,62 @@
 4. in method arguments
 2 ways remain
 ModelAndView sample usage (AddOrganizationController.addOrganization())</t>
+  </si>
+  <si>
+    <t>Session 9</t>
+  </si>
+  <si>
+    <t>Spring MVC using Thymeleaf</t>
+  </si>
+  <si>
+    <t>Spring MVC using lombok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create ProductCategory html page
+</t>
+  </si>
+  <si>
+    <t>08/07/1400</t>
+  </si>
+  <si>
+    <t>Spring Boot</t>
+  </si>
+  <si>
+    <t>produce SOAP and REST Webservices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form:select items
+https://www.baeldung.com/javax-validation
+1. javax-validation-api
+2.hibernate-validator
+3.jakarta-validation
+Validate Product form with default validator annotations
+</t>
+  </si>
+  <si>
+    <t>Session 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Valid vs @Validated
+https://www.baeldung.com/spring-valid-vs-validated
+https://www.baeldung.com/javax-validation-groups
+create custom validator for field level
+review create annotation in java from slides
+@Pattern 
+Regular Expression in java
+https://regex101.com/
+commons validator
+https://commons.apache.org/proper/commons-validator/apidocs/org/apache/commons/validator/routines/package-summary.html#package_description
+create custom validator for class level</t>
+  </si>
+  <si>
+    <t>remove boilerplate code
+Intellj Idea plugins
+create ProductCategory domain
+https://projectlombok.org/features/configuration</t>
+  </si>
+  <si>
+    <t>22/07/1400</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0700D7B-E2DB-4A90-93C9-5BD63601E41E}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +2017,7 @@
         <v>82</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -1979,7 +2032,7 @@
         <v>172</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E60" s="4"/>
     </row>
@@ -1994,45 +2047,108 @@
         <v>83</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
-        <v>8</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+    </row>
+    <row r="65" spans="1:5" ht="269.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="4">
+        <v>9</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D69" t="s">
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D74" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A62:E62"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A20:E20"/>
@@ -2057,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD86837A-08C1-4466-98F6-A3B9221015CB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2085,6 +2201,22 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2094,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0C14A6-F2E4-471F-BBA9-2EEFDE41F762}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
session 11 & 12 added
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anisa Spring\course files\anisa-spring-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3500CDC3-19F8-4721-A055-3DF116E18CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100CBB1B-85AE-4B00-BCAF-6FEAF9C030DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="197">
   <si>
     <t>Session</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>Spring Form Validation</t>
-  </si>
-  <si>
-    <t>Whats new in Spring  5 - Spring MVC</t>
   </si>
   <si>
     <t>Spring JDBC</t>
@@ -690,10 +687,6 @@
     <t>Spring MVC using lombok</t>
   </si>
   <si>
-    <t xml:space="preserve">create ProductCategory html page
-</t>
-  </si>
-  <si>
     <t>08/07/1400</t>
   </si>
   <si>
@@ -735,6 +728,58 @@
   </si>
   <si>
     <t>22/07/1400</t>
+  </si>
+  <si>
+    <t>Session 11</t>
+  </si>
+  <si>
+    <t>some useful notes</t>
+  </si>
+  <si>
+    <t>Create Class for Mappings and Views
+redirect:</t>
+  </si>
+  <si>
+    <t>SpringBoot</t>
+  </si>
+  <si>
+    <t>review Slides</t>
+  </si>
+  <si>
+    <t>Create simple project with Spring Initializr</t>
+  </si>
+  <si>
+    <t>https://start.spring.io/
+display project structure 
+configure Spring boot to support jsp views and create simpl project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intro to thymeleaf
+configuring pom.xml to support thymeleaf
+create simple page
+dev tools dependency
+Thymeleaf Fragments and Decoupled Template Logic
+Template Preprocessing for Mappings constants (not working with thymeleaf 3.0.12+)
+https://www.thymeleaf.org/releasenotes.html#thymeleaf-3.0.12
+</t>
+  </si>
+  <si>
+    <t>Continue with Spring MVC using Thymeleaf</t>
+  </si>
+  <si>
+    <t>Session 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thymeleaf Fragments and Decoupled Template Logic - configuring beanSpringResourceTemplateResolver
+create dummy classes for controller, service and repository for user model
+populate data table by  Decoupled Template Logic technique
+add css resource using thymeleaf
+using  Decoupled Template Logic for fragments
+Spring Internationalization
+type of LocaleResolvers (https://docs.spring.io/spring-framework/docs/current/javadoc-api/org/springframework/web/servlet/LocaleResolver.html)
+file encoding in settings of ide
+Locale Change Interceptor
+</t>
   </si>
 </sst>
 </file>
@@ -1174,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0700D7B-E2DB-4A90-93C9-5BD63601E41E}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -1808,13 +1853,13 @@
         <v>5</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="E44" s="4"/>
     </row>
@@ -1823,45 +1868,45 @@
         <v>5</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -1871,13 +1916,13 @@
     <row r="49" spans="1:5" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="D49" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" s="4"/>
     </row>
@@ -1889,13 +1934,13 @@
         <v>63</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1909,7 +1954,7 @@
         <v>78</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" s="4"/>
     </row>
@@ -1924,7 +1969,7 @@
         <v>69</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="4"/>
     </row>
@@ -1939,7 +1984,7 @@
         <v>79</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E53" s="4"/>
     </row>
@@ -1954,13 +1999,13 @@
         <v>80</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
@@ -1975,10 +2020,10 @@
         <v>80</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>166</v>
       </c>
       <c r="E56" s="4"/>
     </row>
@@ -1993,13 +2038,13 @@
         <v>81</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -2017,7 +2062,7 @@
         <v>82</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E59" s="4"/>
     </row>
@@ -2029,10 +2074,10 @@
         <v>63</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="E60" s="4"/>
     </row>
@@ -2047,13 +2092,13 @@
         <v>83</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
@@ -2071,13 +2116,13 @@
         <v>84</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E63" s="4"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B64" s="16"/>
       <c r="C64" s="16"/>
@@ -2089,11 +2134,11 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>63</v>
@@ -2102,60 +2147,121 @@
         <v>177</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D67" s="10" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E67" s="4"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="4">
-        <v>9</v>
-      </c>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+    </row>
+    <row r="68" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
       <c r="B68" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D68" s="4"/>
+        <v>187</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="E68" s="4"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>181</v>
-      </c>
-      <c r="C73" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D74" t="s">
-        <v>157</v>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+    </row>
+    <row r="73" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="4">
+        <v>9</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D79" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A64:E64"/>
     <mergeCell ref="A62:E62"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{A4A7D2A0-BF27-44D8-8568-97857CB06FB1}"/>
@@ -2175,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD86837A-08C1-4466-98F6-A3B9221015CB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2187,15 +2293,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
         <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>30</v>
@@ -2203,7 +2309,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>240</v>
@@ -2211,7 +2317,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4">
         <v>45</v>
@@ -2248,273 +2354,273 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="J1" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="13"/>
       <c r="D2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" t="s">
-        <v>113</v>
-      </c>
       <c r="H2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" t="s">
         <v>118</v>
       </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
       <c r="J2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="13"/>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="13"/>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="13"/>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="13"/>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="13"/>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="13"/>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="13"/>
       <c r="D9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Session 16 and 17
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anisa Spring\course files\anisa-spring-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B025A1B8-2B07-4815-82CE-471CC7702913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F16AE8F-5E2D-48EB-9E66-43FA91A48C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="233">
   <si>
     <t>Session</t>
   </si>
@@ -846,6 +846,51 @@
   </si>
   <si>
     <t>move properties to configuration file using AppProperties</t>
+  </si>
+  <si>
+    <t>Session 16</t>
+  </si>
+  <si>
+    <t>Support XML and JSON for Request and Response with accept header</t>
+  </si>
+  <si>
+    <t>Update User</t>
+  </si>
+  <si>
+    <t>Session 17</t>
+  </si>
+  <si>
+    <t>Make Custom Exception and CustomErrors</t>
+  </si>
+  <si>
+    <t>Write ControllerAdvice for handle errors</t>
+  </si>
+  <si>
+    <t>Results Pagination for getAll using PagingAndSortingRepository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create contextpath and Build jar file and </t>
+  </si>
+  <si>
+    <t>Create war file - SpringBootServletInitializer, tomcat as provider</t>
+  </si>
+  <si>
+    <t>make tomcat server</t>
+  </si>
+  <si>
+    <t>SOAP</t>
+  </si>
+  <si>
+    <t>Rest Client</t>
+  </si>
+  <si>
+    <t>RestClient</t>
+  </si>
+  <si>
+    <t>SOAP Server And Client</t>
+  </si>
+  <si>
+    <t>Session 18</t>
   </si>
 </sst>
 </file>
@@ -892,7 +937,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -908,6 +953,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -934,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -973,6 +1024,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1288,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0700D7B-E2DB-4A90-93C9-5BD63601E41E}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2423,28 +2475,118 @@
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D93" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D94" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D96" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D98" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D99" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D100" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D101" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D104" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B101" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>202</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B110" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A67:E67"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A43:E43"/>
@@ -2454,11 +2596,11 @@
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A92:E92"/>
+    <mergeCell ref="A95:E95"/>
     <mergeCell ref="A77:E77"/>
     <mergeCell ref="A84:E84"/>
     <mergeCell ref="A74:E74"/>
-    <mergeCell ref="A72:E72"/>
-    <mergeCell ref="A67:E67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{A4A7D2A0-BF27-44D8-8568-97857CB06FB1}"/>

</xml_diff>

<commit_message>
Session 24 added - Spring Boot Security ACL
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anisa Spring\course files\anisa-spring-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86904E18-B16D-4C5E-B8D2-72FB7FF5A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2BA726-5651-4957-A2D5-C96761ACB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="244">
   <si>
     <t>Session</t>
   </si>
@@ -794,9 +794,6 @@
     <t>Security</t>
   </si>
   <si>
-    <t>Microservice</t>
-  </si>
-  <si>
     <t>Cloud</t>
   </si>
   <si>
@@ -909,6 +906,27 @@
   </si>
   <si>
     <t>Spring Batch</t>
+  </si>
+  <si>
+    <t>Spring Security ACL</t>
+  </si>
+  <si>
+    <t>https://github.com/spring-projects/spring-security/blob/main/acl/src/main/java/org/springframework/security/acls/domain/BasePermission.java</t>
+  </si>
+  <si>
+    <t>https://www.baeldung.com/spring-security-acl</t>
+  </si>
+  <si>
+    <t>Microservice, docker, kubernetes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GTln3jc5_eg</t>
+  </si>
+  <si>
+    <t>Session 24</t>
+  </si>
+  <si>
+    <t>Session 25</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0700D7B-E2DB-4A90-93C9-5BD63601E41E}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,7 +2416,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -2407,18 +2425,18 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C78" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C79" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2426,7 +2444,7 @@
         <v>200</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2434,17 +2452,17 @@
         <v>200</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D82" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -2453,42 +2471,42 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D85" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -2497,17 +2515,17 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D93" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D94" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -2516,37 +2534,37 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D96" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D99" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D100" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D101" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -2555,20 +2573,20 @@
     </row>
     <row r="103" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
@@ -2576,48 +2594,92 @@
       <c r="E105" s="17"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B106" t="s">
-        <v>199</v>
-      </c>
       <c r="C106" t="s">
         <v>200</v>
       </c>
       <c r="D106" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B107" s="17"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D108" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D110" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D111" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B112" s="17"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="17"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B108" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B110" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B112" t="s">
-        <v>237</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A112:E112"/>
     <mergeCell ref="A105:E105"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A32:E32"/>
@@ -2634,8 +2696,6 @@
     <mergeCell ref="A72:E72"/>
     <mergeCell ref="A67:E67"/>
     <mergeCell ref="A92:E92"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A77:E77"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{A4A7D2A0-BF27-44D8-8568-97857CB06FB1}"/>

</xml_diff>

<commit_message>
session 25 and 26 added
</commit_message>
<xml_diff>
--- a/syllabus.xlsx
+++ b/syllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anisa Spring\course files\anisa-spring-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2BA726-5651-4957-A2D5-C96761ACB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740107F7-8E69-401F-ADFB-6B3E9817EA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{964B4250-0E44-43A3-827A-148A57DAA8FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="254">
   <si>
     <t>Session</t>
   </si>
@@ -927,6 +927,37 @@
   </si>
   <si>
     <t>Session 25</t>
+  </si>
+  <si>
+    <t>Rest Assured</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>gherkin</t>
+  </si>
+  <si>
+    <t>https://www.baeldung.com/junit-5-repeated-test</t>
+  </si>
+  <si>
+    <t>Session 26</t>
+  </si>
+  <si>
+    <t>https://www.baeldung.com/spring-boot-h2-database</t>
+  </si>
+  <si>
+    <t>jUnit repeat test</t>
+  </si>
+  <si>
+    <t>H2 Database in memory</t>
+  </si>
+  <si>
+    <t>https://rest-assured.io/
+https://maven.apache.org/surefire/maven-surefire-plugin/</t>
+  </si>
+  <si>
+    <t>Junit 5 and Mockito</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0700D7B-E2DB-4A90-93C9-5BD63601E41E}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2639,48 +2670,91 @@
       <c r="D112" s="17"/>
       <c r="E112" s="17"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B118" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D113" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C115" t="s">
+        <v>250</v>
+      </c>
+      <c r="D115" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C116" t="s">
+        <v>251</v>
+      </c>
+      <c r="D116" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C117" t="s">
+        <v>244</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D118" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D119" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B119" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A77:E77"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A105:E105"/>
+  <mergeCells count="21">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A43:E43"/>
@@ -2690,12 +2764,18 @@
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A114:E114"/>
     <mergeCell ref="A74:E74"/>
     <mergeCell ref="A102:E102"/>
     <mergeCell ref="A72:E72"/>
     <mergeCell ref="A67:E67"/>
     <mergeCell ref="A92:E92"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A105:E105"/>
+    <mergeCell ref="A84:E84"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{A4A7D2A0-BF27-44D8-8568-97857CB06FB1}"/>

</xml_diff>